<commit_message>
added scatterplot with test data
</commit_message>
<xml_diff>
--- a/Data_species_landcover_lebensqualitaet.xlsx
+++ b/Data_species_landcover_lebensqualitaet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karin.guedel@fhnw.ch/WebstormProjects/guedelkohler/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5A555C5-3452-424E-9F1C-24D9F5302322}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D34D4160-FE64-6740-8B0F-CE0EC6B71E65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15840" xr2:uid="{D2388905-A8AE-974C-BCD5-3987D3404137}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15840" activeTab="2" xr2:uid="{D2388905-A8AE-974C-BCD5-3987D3404137}"/>
   </bookViews>
   <sheets>
     <sheet name="alle_Daten&amp;ersteBerechnungen" sheetId="1" r:id="rId1"/>
@@ -1361,6 +1361,12 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -1376,6 +1382,18 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1384,24 +1402,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2020,6 +2020,63 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="de-DE"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:trendline>
             <c:spPr>
               <a:ln w="19050" cap="rnd">
@@ -6902,7 +6959,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B87E9FEC-8EB8-C841-9A32-0C14DA21BCFE}">
   <dimension ref="A2:DF242"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BZ13" workbookViewId="0">
+    <sheetView topLeftCell="BY12" workbookViewId="0">
       <selection activeCell="BB1" sqref="BB1:BO1048576"/>
     </sheetView>
   </sheetViews>
@@ -6925,60 +6982,60 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:110" ht="51" x14ac:dyDescent="0.2">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="35" t="s">
         <v>286</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="41" t="s">
+      <c r="B2" s="36"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="42" t="s">
         <v>251</v>
       </c>
-      <c r="E2" s="42"/>
-      <c r="F2" s="41" t="s">
+      <c r="E2" s="43"/>
+      <c r="F2" s="42" t="s">
         <v>252</v>
       </c>
-      <c r="G2" s="42"/>
-      <c r="H2" s="41" t="s">
+      <c r="G2" s="43"/>
+      <c r="H2" s="42" t="s">
         <v>253</v>
       </c>
-      <c r="I2" s="42"/>
-      <c r="J2" s="41" t="s">
+      <c r="I2" s="43"/>
+      <c r="J2" s="42" t="s">
         <v>254</v>
       </c>
-      <c r="K2" s="42"/>
-      <c r="L2" s="41" t="s">
+      <c r="K2" s="43"/>
+      <c r="L2" s="42" t="s">
         <v>255</v>
       </c>
-      <c r="M2" s="42"/>
-      <c r="N2" s="41" t="s">
+      <c r="M2" s="43"/>
+      <c r="N2" s="42" t="s">
         <v>256</v>
       </c>
-      <c r="O2" s="42"/>
-      <c r="P2" s="41" t="s">
+      <c r="O2" s="43"/>
+      <c r="P2" s="42" t="s">
         <v>257</v>
       </c>
-      <c r="Q2" s="42"/>
-      <c r="R2" s="41" t="s">
+      <c r="Q2" s="43"/>
+      <c r="R2" s="42" t="s">
         <v>258</v>
       </c>
-      <c r="S2" s="42"/>
-      <c r="T2" s="41" t="s">
+      <c r="S2" s="43"/>
+      <c r="T2" s="42" t="s">
         <v>259</v>
       </c>
-      <c r="U2" s="42"/>
-      <c r="V2" s="41" t="s">
+      <c r="U2" s="43"/>
+      <c r="V2" s="42" t="s">
         <v>260</v>
       </c>
-      <c r="W2" s="42"/>
-      <c r="X2" s="41" t="s">
+      <c r="W2" s="43"/>
+      <c r="X2" s="42" t="s">
         <v>261</v>
       </c>
-      <c r="Y2" s="42"/>
-      <c r="Z2" s="33" t="s">
+      <c r="Y2" s="43"/>
+      <c r="Z2" s="35" t="s">
         <v>302</v>
       </c>
-      <c r="AA2" s="34"/>
-      <c r="AB2" s="35"/>
+      <c r="AA2" s="36"/>
+      <c r="AB2" s="37"/>
       <c r="AC2" s="1" t="s">
         <v>0</v>
       </c>
@@ -7006,11 +7063,11 @@
       <c r="AK2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="AL2" s="33" t="s">
+      <c r="AL2" s="35" t="s">
         <v>303</v>
       </c>
-      <c r="AM2" s="34"/>
-      <c r="AN2" s="35"/>
+      <c r="AM2" s="36"/>
+      <c r="AN2" s="37"/>
       <c r="AO2" s="1" t="s">
         <v>0</v>
       </c>
@@ -7047,11 +7104,11 @@
       <c r="AZ2" s="19" t="s">
         <v>293</v>
       </c>
-      <c r="BA2" s="33" t="s">
+      <c r="BA2" s="35" t="s">
         <v>264</v>
       </c>
-      <c r="BB2" s="34"/>
-      <c r="BC2" s="35"/>
+      <c r="BB2" s="36"/>
+      <c r="BC2" s="37"/>
       <c r="BD2" s="1" t="s">
         <v>251</v>
       </c>
@@ -7085,11 +7142,11 @@
       <c r="BN2" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="BP2" s="33" t="s">
+      <c r="BP2" s="35" t="s">
         <v>265</v>
       </c>
-      <c r="BQ2" s="34"/>
-      <c r="BR2" s="35"/>
+      <c r="BQ2" s="36"/>
+      <c r="BR2" s="37"/>
       <c r="BS2" s="1" t="s">
         <v>251</v>
       </c>
@@ -7167,61 +7224,61 @@
       </c>
     </row>
     <row r="3" spans="1:110" ht="18" x14ac:dyDescent="0.2">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="37"/>
+      <c r="B3" s="39"/>
       <c r="C3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="45" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="46"/>
-      <c r="F3" s="45" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="46"/>
-      <c r="H3" s="45" t="s">
-        <v>10</v>
-      </c>
-      <c r="I3" s="46"/>
-      <c r="J3" s="45" t="s">
-        <v>10</v>
-      </c>
-      <c r="K3" s="46"/>
-      <c r="L3" s="45" t="s">
-        <v>10</v>
-      </c>
-      <c r="M3" s="46"/>
-      <c r="N3" s="45" t="s">
-        <v>10</v>
-      </c>
-      <c r="O3" s="46"/>
-      <c r="P3" s="45" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q3" s="46"/>
-      <c r="R3" s="45" t="s">
-        <v>10</v>
-      </c>
-      <c r="S3" s="46"/>
-      <c r="T3" s="45" t="s">
-        <v>10</v>
-      </c>
-      <c r="U3" s="46"/>
-      <c r="V3" s="45" t="s">
-        <v>10</v>
-      </c>
-      <c r="W3" s="46"/>
-      <c r="X3" s="45" t="s">
-        <v>10</v>
-      </c>
-      <c r="Y3" s="46"/>
-      <c r="Z3" s="36" t="s">
+      <c r="D3" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="41"/>
+      <c r="F3" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="41"/>
+      <c r="H3" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" s="41"/>
+      <c r="J3" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="K3" s="41"/>
+      <c r="L3" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="M3" s="41"/>
+      <c r="N3" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="O3" s="41"/>
+      <c r="P3" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q3" s="41"/>
+      <c r="R3" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="S3" s="41"/>
+      <c r="T3" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="U3" s="41"/>
+      <c r="V3" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="W3" s="41"/>
+      <c r="X3" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y3" s="41"/>
+      <c r="Z3" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="AA3" s="37"/>
+      <c r="AA3" s="39"/>
       <c r="AB3" s="3" t="s">
         <v>10</v>
       </c>
@@ -7252,10 +7309,10 @@
       <c r="AK3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="AL3" s="36" t="s">
+      <c r="AL3" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="AM3" s="37"/>
+      <c r="AM3" s="39"/>
       <c r="AN3" s="3" t="s">
         <v>10</v>
       </c>
@@ -7286,10 +7343,10 @@
       <c r="AW3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="BA3" s="36" t="s">
+      <c r="BA3" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="BB3" s="37"/>
+      <c r="BB3" s="39"/>
       <c r="BC3" s="3" t="s">
         <v>10</v>
       </c>
@@ -7326,10 +7383,10 @@
       <c r="BN3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="BP3" s="36" t="s">
+      <c r="BP3" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="BQ3" s="37"/>
+      <c r="BQ3" s="39"/>
       <c r="BR3" s="3" t="s">
         <v>10</v>
       </c>
@@ -11491,10 +11548,10 @@
       <c r="DF15" s="16"/>
     </row>
     <row r="16" spans="1:110" ht="18" x14ac:dyDescent="0.2">
-      <c r="A16" s="43" t="s">
+      <c r="A16" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="44"/>
+      <c r="B16" s="34"/>
       <c r="C16" s="3" t="s">
         <v>10</v>
       </c>
@@ -11564,10 +11621,10 @@
       <c r="Y16" s="12">
         <v>35.959000000000003</v>
       </c>
-      <c r="Z16" s="43" t="s">
+      <c r="Z16" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="AA16" s="44"/>
+      <c r="AA16" s="34"/>
       <c r="AB16" s="3" t="s">
         <v>10</v>
       </c>
@@ -11598,10 +11655,10 @@
       <c r="AK16" s="6">
         <v>1.2414831151000001</v>
       </c>
-      <c r="AL16" s="43" t="s">
+      <c r="AL16" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="AM16" s="44"/>
+      <c r="AM16" s="34"/>
       <c r="AN16" s="3" t="s">
         <v>10</v>
       </c>
@@ -11644,10 +11701,10 @@
         <f t="shared" si="6"/>
         <v>0.3239488917663188</v>
       </c>
-      <c r="BA16" s="43" t="s">
+      <c r="BA16" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="BB16" s="44"/>
+      <c r="BB16" s="34"/>
       <c r="BC16" s="3" t="s">
         <v>10</v>
       </c>
@@ -11688,10 +11745,10 @@
         <f t="shared" si="7"/>
         <v>19129</v>
       </c>
-      <c r="BP16" s="43" t="s">
+      <c r="BP16" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="BQ16" s="44"/>
+      <c r="BQ16" s="34"/>
       <c r="BR16" s="3" t="s">
         <v>10</v>
       </c>
@@ -19911,7 +19968,7 @@
       <c r="DF45" s="16"/>
     </row>
     <row r="46" spans="1:110" ht="18" x14ac:dyDescent="0.2">
-      <c r="Z46" s="38" t="s">
+      <c r="Z46" s="44" t="s">
         <v>53</v>
       </c>
       <c r="AA46" s="9" t="s">
@@ -19960,7 +20017,7 @@
       <c r="DF46" s="16"/>
     </row>
     <row r="47" spans="1:110" ht="18" x14ac:dyDescent="0.2">
-      <c r="Z47" s="39"/>
+      <c r="Z47" s="45"/>
       <c r="AA47" s="9" t="s">
         <v>55</v>
       </c>
@@ -20007,7 +20064,7 @@
       <c r="DF47" s="16"/>
     </row>
     <row r="48" spans="1:110" ht="18" x14ac:dyDescent="0.2">
-      <c r="Z48" s="39"/>
+      <c r="Z48" s="45"/>
       <c r="AA48" s="9" t="s">
         <v>56</v>
       </c>
@@ -20054,7 +20111,7 @@
       <c r="DF48" s="16"/>
     </row>
     <row r="49" spans="26:110" ht="24" x14ac:dyDescent="0.2">
-      <c r="Z49" s="39"/>
+      <c r="Z49" s="45"/>
       <c r="AA49" s="9" t="s">
         <v>57</v>
       </c>
@@ -20101,7 +20158,7 @@
       <c r="DF49" s="16"/>
     </row>
     <row r="50" spans="26:110" ht="18" x14ac:dyDescent="0.2">
-      <c r="Z50" s="39"/>
+      <c r="Z50" s="45"/>
       <c r="AA50" s="9" t="s">
         <v>58</v>
       </c>
@@ -20148,7 +20205,7 @@
       <c r="DF50" s="16"/>
     </row>
     <row r="51" spans="26:110" ht="18" x14ac:dyDescent="0.2">
-      <c r="Z51" s="39"/>
+      <c r="Z51" s="45"/>
       <c r="AA51" s="9" t="s">
         <v>59</v>
       </c>
@@ -20195,7 +20252,7 @@
       <c r="DF51" s="16"/>
     </row>
     <row r="52" spans="26:110" ht="18" x14ac:dyDescent="0.2">
-      <c r="Z52" s="39"/>
+      <c r="Z52" s="45"/>
       <c r="AA52" s="9" t="s">
         <v>60</v>
       </c>
@@ -20242,7 +20299,7 @@
       <c r="DF52" s="16"/>
     </row>
     <row r="53" spans="26:110" ht="18" x14ac:dyDescent="0.2">
-      <c r="Z53" s="39"/>
+      <c r="Z53" s="45"/>
       <c r="AA53" s="9" t="s">
         <v>61</v>
       </c>
@@ -20289,7 +20346,7 @@
       <c r="DF53" s="16"/>
     </row>
     <row r="54" spans="26:110" ht="24" x14ac:dyDescent="0.2">
-      <c r="Z54" s="39"/>
+      <c r="Z54" s="45"/>
       <c r="AA54" s="9" t="s">
         <v>62</v>
       </c>
@@ -20336,7 +20393,7 @@
       <c r="DF54" s="16"/>
     </row>
     <row r="55" spans="26:110" ht="18" x14ac:dyDescent="0.2">
-      <c r="Z55" s="39"/>
+      <c r="Z55" s="45"/>
       <c r="AA55" s="9" t="s">
         <v>63</v>
       </c>
@@ -20383,7 +20440,7 @@
       <c r="DF55" s="16"/>
     </row>
     <row r="56" spans="26:110" ht="18" x14ac:dyDescent="0.2">
-      <c r="Z56" s="39"/>
+      <c r="Z56" s="45"/>
       <c r="AA56" s="10" t="s">
         <v>64</v>
       </c>
@@ -20430,7 +20487,7 @@
       <c r="DF56" s="16"/>
     </row>
     <row r="57" spans="26:110" ht="18" x14ac:dyDescent="0.2">
-      <c r="Z57" s="39"/>
+      <c r="Z57" s="45"/>
       <c r="AA57" s="10" t="s">
         <v>65</v>
       </c>
@@ -20477,7 +20534,7 @@
       <c r="DF57" s="16"/>
     </row>
     <row r="58" spans="26:110" ht="18" x14ac:dyDescent="0.2">
-      <c r="Z58" s="39"/>
+      <c r="Z58" s="45"/>
       <c r="AA58" s="10" t="s">
         <v>66</v>
       </c>
@@ -20524,7 +20581,7 @@
       <c r="DF58" s="16"/>
     </row>
     <row r="59" spans="26:110" ht="18" x14ac:dyDescent="0.2">
-      <c r="Z59" s="39"/>
+      <c r="Z59" s="45"/>
       <c r="AA59" s="9" t="s">
         <v>67</v>
       </c>
@@ -20571,7 +20628,7 @@
       <c r="DF59" s="16"/>
     </row>
     <row r="60" spans="26:110" ht="18" x14ac:dyDescent="0.2">
-      <c r="Z60" s="39"/>
+      <c r="Z60" s="45"/>
       <c r="AA60" s="9" t="s">
         <v>68</v>
       </c>
@@ -20618,7 +20675,7 @@
       <c r="DF60" s="16"/>
     </row>
     <row r="61" spans="26:110" ht="18" x14ac:dyDescent="0.2">
-      <c r="Z61" s="39"/>
+      <c r="Z61" s="45"/>
       <c r="AA61" s="9" t="s">
         <v>69</v>
       </c>
@@ -20665,7 +20722,7 @@
       <c r="DF61" s="16"/>
     </row>
     <row r="62" spans="26:110" ht="18" x14ac:dyDescent="0.2">
-      <c r="Z62" s="39"/>
+      <c r="Z62" s="45"/>
       <c r="AA62" s="9" t="s">
         <v>70</v>
       </c>
@@ -20712,7 +20769,7 @@
       <c r="DF62" s="16"/>
     </row>
     <row r="63" spans="26:110" ht="18" x14ac:dyDescent="0.2">
-      <c r="Z63" s="39"/>
+      <c r="Z63" s="45"/>
       <c r="AA63" s="9" t="s">
         <v>71</v>
       </c>
@@ -20759,7 +20816,7 @@
       <c r="DF63" s="16"/>
     </row>
     <row r="64" spans="26:110" ht="18" x14ac:dyDescent="0.2">
-      <c r="Z64" s="39"/>
+      <c r="Z64" s="45"/>
       <c r="AA64" s="9" t="s">
         <v>72</v>
       </c>
@@ -20806,7 +20863,7 @@
       <c r="DF64" s="16"/>
     </row>
     <row r="65" spans="26:110" ht="18" x14ac:dyDescent="0.2">
-      <c r="Z65" s="39"/>
+      <c r="Z65" s="45"/>
       <c r="AA65" s="9" t="s">
         <v>73</v>
       </c>
@@ -20853,7 +20910,7 @@
       <c r="DF65" s="16"/>
     </row>
     <row r="66" spans="26:110" ht="18" x14ac:dyDescent="0.2">
-      <c r="Z66" s="39"/>
+      <c r="Z66" s="45"/>
       <c r="AA66" s="9" t="s">
         <v>74</v>
       </c>
@@ -20900,7 +20957,7 @@
       <c r="DF66" s="16"/>
     </row>
     <row r="67" spans="26:110" ht="18" x14ac:dyDescent="0.2">
-      <c r="Z67" s="39"/>
+      <c r="Z67" s="45"/>
       <c r="AA67" s="9" t="s">
         <v>75</v>
       </c>
@@ -20947,7 +21004,7 @@
       <c r="DF67" s="16"/>
     </row>
     <row r="68" spans="26:110" ht="18" x14ac:dyDescent="0.2">
-      <c r="Z68" s="39"/>
+      <c r="Z68" s="45"/>
       <c r="AA68" s="9" t="s">
         <v>76</v>
       </c>
@@ -20994,7 +21051,7 @@
       <c r="DF68" s="16"/>
     </row>
     <row r="69" spans="26:110" ht="24" x14ac:dyDescent="0.2">
-      <c r="Z69" s="39"/>
+      <c r="Z69" s="45"/>
       <c r="AA69" s="10" t="s">
         <v>77</v>
       </c>
@@ -21041,7 +21098,7 @@
       <c r="DF69" s="16"/>
     </row>
     <row r="70" spans="26:110" ht="18" x14ac:dyDescent="0.2">
-      <c r="Z70" s="39"/>
+      <c r="Z70" s="45"/>
       <c r="AA70" s="9" t="s">
         <v>78</v>
       </c>
@@ -21088,7 +21145,7 @@
       <c r="DF70" s="16"/>
     </row>
     <row r="71" spans="26:110" ht="24" x14ac:dyDescent="0.2">
-      <c r="Z71" s="39"/>
+      <c r="Z71" s="45"/>
       <c r="AA71" s="9" t="s">
         <v>79</v>
       </c>
@@ -21135,7 +21192,7 @@
       <c r="DF71" s="16"/>
     </row>
     <row r="72" spans="26:110" ht="18" x14ac:dyDescent="0.2">
-      <c r="Z72" s="39"/>
+      <c r="Z72" s="45"/>
       <c r="AA72" s="9" t="s">
         <v>80</v>
       </c>
@@ -21182,7 +21239,7 @@
       <c r="DF72" s="16"/>
     </row>
     <row r="73" spans="26:110" ht="36" x14ac:dyDescent="0.2">
-      <c r="Z73" s="39"/>
+      <c r="Z73" s="45"/>
       <c r="AA73" s="9" t="s">
         <v>81</v>
       </c>
@@ -21229,7 +21286,7 @@
       <c r="DF73" s="16"/>
     </row>
     <row r="74" spans="26:110" ht="24" x14ac:dyDescent="0.2">
-      <c r="Z74" s="39"/>
+      <c r="Z74" s="45"/>
       <c r="AA74" s="9" t="s">
         <v>82</v>
       </c>
@@ -21276,7 +21333,7 @@
       <c r="DF74" s="16"/>
     </row>
     <row r="75" spans="26:110" ht="24" x14ac:dyDescent="0.2">
-      <c r="Z75" s="39"/>
+      <c r="Z75" s="45"/>
       <c r="AA75" s="9" t="s">
         <v>83</v>
       </c>
@@ -21323,7 +21380,7 @@
       <c r="DF75" s="16"/>
     </row>
     <row r="76" spans="26:110" ht="18" x14ac:dyDescent="0.2">
-      <c r="Z76" s="39"/>
+      <c r="Z76" s="45"/>
       <c r="AA76" s="9" t="s">
         <v>84</v>
       </c>
@@ -21370,7 +21427,7 @@
       <c r="DF76" s="16"/>
     </row>
     <row r="77" spans="26:110" ht="18" x14ac:dyDescent="0.2">
-      <c r="Z77" s="39"/>
+      <c r="Z77" s="45"/>
       <c r="AA77" s="10" t="s">
         <v>85</v>
       </c>
@@ -21417,7 +21474,7 @@
       <c r="DF77" s="16"/>
     </row>
     <row r="78" spans="26:110" ht="18" x14ac:dyDescent="0.2">
-      <c r="Z78" s="39"/>
+      <c r="Z78" s="45"/>
       <c r="AA78" s="9" t="s">
         <v>86</v>
       </c>
@@ -21464,7 +21521,7 @@
       <c r="DF78" s="16"/>
     </row>
     <row r="79" spans="26:110" ht="18" x14ac:dyDescent="0.2">
-      <c r="Z79" s="39"/>
+      <c r="Z79" s="45"/>
       <c r="AA79" s="10" t="s">
         <v>87</v>
       </c>
@@ -21511,7 +21568,7 @@
       <c r="DF79" s="16"/>
     </row>
     <row r="80" spans="26:110" ht="18" x14ac:dyDescent="0.2">
-      <c r="Z80" s="39"/>
+      <c r="Z80" s="45"/>
       <c r="AA80" s="9" t="s">
         <v>88</v>
       </c>
@@ -21558,7 +21615,7 @@
       <c r="DF80" s="16"/>
     </row>
     <row r="81" spans="26:110" ht="18" x14ac:dyDescent="0.2">
-      <c r="Z81" s="39"/>
+      <c r="Z81" s="45"/>
       <c r="AA81" s="9" t="s">
         <v>89</v>
       </c>
@@ -21605,7 +21662,7 @@
       <c r="DF81" s="16"/>
     </row>
     <row r="82" spans="26:110" ht="24" x14ac:dyDescent="0.2">
-      <c r="Z82" s="39"/>
+      <c r="Z82" s="45"/>
       <c r="AA82" s="9" t="s">
         <v>90</v>
       </c>
@@ -21652,7 +21709,7 @@
       <c r="DF82" s="16"/>
     </row>
     <row r="83" spans="26:110" ht="36" x14ac:dyDescent="0.2">
-      <c r="Z83" s="39"/>
+      <c r="Z83" s="45"/>
       <c r="AA83" s="9" t="s">
         <v>91</v>
       </c>
@@ -21699,7 +21756,7 @@
       <c r="DF83" s="16"/>
     </row>
     <row r="84" spans="26:110" ht="18" x14ac:dyDescent="0.2">
-      <c r="Z84" s="39"/>
+      <c r="Z84" s="45"/>
       <c r="AA84" s="9" t="s">
         <v>92</v>
       </c>
@@ -21746,7 +21803,7 @@
       <c r="DF84" s="16"/>
     </row>
     <row r="85" spans="26:110" ht="36" x14ac:dyDescent="0.2">
-      <c r="Z85" s="39"/>
+      <c r="Z85" s="45"/>
       <c r="AA85" s="9" t="s">
         <v>93</v>
       </c>
@@ -21793,7 +21850,7 @@
       <c r="DF85" s="16"/>
     </row>
     <row r="86" spans="26:110" ht="24" x14ac:dyDescent="0.2">
-      <c r="Z86" s="39"/>
+      <c r="Z86" s="45"/>
       <c r="AA86" s="9" t="s">
         <v>94</v>
       </c>
@@ -21840,7 +21897,7 @@
       <c r="DF86" s="16"/>
     </row>
     <row r="87" spans="26:110" ht="36" x14ac:dyDescent="0.2">
-      <c r="Z87" s="39"/>
+      <c r="Z87" s="45"/>
       <c r="AA87" s="9" t="s">
         <v>95</v>
       </c>
@@ -21887,7 +21944,7 @@
       <c r="DF87" s="16"/>
     </row>
     <row r="88" spans="26:110" ht="18" x14ac:dyDescent="0.2">
-      <c r="Z88" s="39"/>
+      <c r="Z88" s="45"/>
       <c r="AA88" s="9" t="s">
         <v>96</v>
       </c>
@@ -21934,7 +21991,7 @@
       <c r="DF88" s="16"/>
     </row>
     <row r="89" spans="26:110" ht="18" x14ac:dyDescent="0.2">
-      <c r="Z89" s="39"/>
+      <c r="Z89" s="45"/>
       <c r="AA89" s="9" t="s">
         <v>97</v>
       </c>
@@ -21981,7 +22038,7 @@
       <c r="DF89" s="16"/>
     </row>
     <row r="90" spans="26:110" ht="36" x14ac:dyDescent="0.2">
-      <c r="Z90" s="39"/>
+      <c r="Z90" s="45"/>
       <c r="AA90" s="10" t="s">
         <v>98</v>
       </c>
@@ -22017,7 +22074,7 @@
       </c>
     </row>
     <row r="91" spans="26:110" x14ac:dyDescent="0.2">
-      <c r="Z91" s="39"/>
+      <c r="Z91" s="45"/>
       <c r="AA91" s="9" t="s">
         <v>99</v>
       </c>
@@ -22053,7 +22110,7 @@
       </c>
     </row>
     <row r="92" spans="26:110" x14ac:dyDescent="0.2">
-      <c r="Z92" s="39"/>
+      <c r="Z92" s="45"/>
       <c r="AA92" s="10" t="s">
         <v>100</v>
       </c>
@@ -22089,7 +22146,7 @@
       </c>
     </row>
     <row r="93" spans="26:110" x14ac:dyDescent="0.2">
-      <c r="Z93" s="39"/>
+      <c r="Z93" s="45"/>
       <c r="AA93" s="9" t="s">
         <v>101</v>
       </c>
@@ -22125,7 +22182,7 @@
       </c>
     </row>
     <row r="94" spans="26:110" x14ac:dyDescent="0.2">
-      <c r="Z94" s="39"/>
+      <c r="Z94" s="45"/>
       <c r="AA94" s="9" t="s">
         <v>102</v>
       </c>
@@ -22161,7 +22218,7 @@
       </c>
     </row>
     <row r="95" spans="26:110" x14ac:dyDescent="0.2">
-      <c r="Z95" s="39"/>
+      <c r="Z95" s="45"/>
       <c r="AA95" s="10" t="s">
         <v>103</v>
       </c>
@@ -22197,7 +22254,7 @@
       </c>
     </row>
     <row r="96" spans="26:110" x14ac:dyDescent="0.2">
-      <c r="Z96" s="39"/>
+      <c r="Z96" s="45"/>
       <c r="AA96" s="9" t="s">
         <v>104</v>
       </c>
@@ -22233,7 +22290,7 @@
       </c>
     </row>
     <row r="97" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z97" s="39"/>
+      <c r="Z97" s="45"/>
       <c r="AA97" s="9" t="s">
         <v>105</v>
       </c>
@@ -22269,7 +22326,7 @@
       </c>
     </row>
     <row r="98" spans="26:37" ht="24" x14ac:dyDescent="0.2">
-      <c r="Z98" s="39"/>
+      <c r="Z98" s="45"/>
       <c r="AA98" s="9" t="s">
         <v>106</v>
       </c>
@@ -22305,7 +22362,7 @@
       </c>
     </row>
     <row r="99" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z99" s="39"/>
+      <c r="Z99" s="45"/>
       <c r="AA99" s="9" t="s">
         <v>107</v>
       </c>
@@ -22341,7 +22398,7 @@
       </c>
     </row>
     <row r="100" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z100" s="39"/>
+      <c r="Z100" s="45"/>
       <c r="AA100" s="9" t="s">
         <v>108</v>
       </c>
@@ -22377,7 +22434,7 @@
       </c>
     </row>
     <row r="101" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z101" s="39"/>
+      <c r="Z101" s="45"/>
       <c r="AA101" s="9" t="s">
         <v>109</v>
       </c>
@@ -22413,7 +22470,7 @@
       </c>
     </row>
     <row r="102" spans="26:37" ht="24" x14ac:dyDescent="0.2">
-      <c r="Z102" s="39"/>
+      <c r="Z102" s="45"/>
       <c r="AA102" s="9" t="s">
         <v>110</v>
       </c>
@@ -22449,7 +22506,7 @@
       </c>
     </row>
     <row r="103" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z103" s="39"/>
+      <c r="Z103" s="45"/>
       <c r="AA103" s="10" t="s">
         <v>111</v>
       </c>
@@ -22485,7 +22542,7 @@
       </c>
     </row>
     <row r="104" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z104" s="39"/>
+      <c r="Z104" s="45"/>
       <c r="AA104" s="10" t="s">
         <v>112</v>
       </c>
@@ -22521,7 +22578,7 @@
       </c>
     </row>
     <row r="105" spans="26:37" ht="24" x14ac:dyDescent="0.2">
-      <c r="Z105" s="39"/>
+      <c r="Z105" s="45"/>
       <c r="AA105" s="9" t="s">
         <v>113</v>
       </c>
@@ -22557,7 +22614,7 @@
       </c>
     </row>
     <row r="106" spans="26:37" ht="36" x14ac:dyDescent="0.2">
-      <c r="Z106" s="39"/>
+      <c r="Z106" s="45"/>
       <c r="AA106" s="9" t="s">
         <v>114</v>
       </c>
@@ -22593,7 +22650,7 @@
       </c>
     </row>
     <row r="107" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z107" s="39"/>
+      <c r="Z107" s="45"/>
       <c r="AA107" s="9" t="s">
         <v>115</v>
       </c>
@@ -22629,7 +22686,7 @@
       </c>
     </row>
     <row r="108" spans="26:37" ht="24" x14ac:dyDescent="0.2">
-      <c r="Z108" s="39"/>
+      <c r="Z108" s="45"/>
       <c r="AA108" s="9" t="s">
         <v>116</v>
       </c>
@@ -22665,7 +22722,7 @@
       </c>
     </row>
     <row r="109" spans="26:37" ht="48" x14ac:dyDescent="0.2">
-      <c r="Z109" s="39"/>
+      <c r="Z109" s="45"/>
       <c r="AA109" s="9" t="s">
         <v>117</v>
       </c>
@@ -22701,7 +22758,7 @@
       </c>
     </row>
     <row r="110" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z110" s="39"/>
+      <c r="Z110" s="45"/>
       <c r="AA110" s="9" t="s">
         <v>118</v>
       </c>
@@ -22737,7 +22794,7 @@
       </c>
     </row>
     <row r="111" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z111" s="39"/>
+      <c r="Z111" s="45"/>
       <c r="AA111" s="9" t="s">
         <v>119</v>
       </c>
@@ -22773,7 +22830,7 @@
       </c>
     </row>
     <row r="112" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z112" s="39"/>
+      <c r="Z112" s="45"/>
       <c r="AA112" s="10" t="s">
         <v>120</v>
       </c>
@@ -22809,7 +22866,7 @@
       </c>
     </row>
     <row r="113" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z113" s="39"/>
+      <c r="Z113" s="45"/>
       <c r="AA113" s="9" t="s">
         <v>121</v>
       </c>
@@ -22845,7 +22902,7 @@
       </c>
     </row>
     <row r="114" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z114" s="39"/>
+      <c r="Z114" s="45"/>
       <c r="AA114" s="9" t="s">
         <v>122</v>
       </c>
@@ -22881,7 +22938,7 @@
       </c>
     </row>
     <row r="115" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z115" s="39"/>
+      <c r="Z115" s="45"/>
       <c r="AA115" s="9" t="s">
         <v>123</v>
       </c>
@@ -22917,7 +22974,7 @@
       </c>
     </row>
     <row r="116" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z116" s="39"/>
+      <c r="Z116" s="45"/>
       <c r="AA116" s="9" t="s">
         <v>124</v>
       </c>
@@ -22953,7 +23010,7 @@
       </c>
     </row>
     <row r="117" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z117" s="39"/>
+      <c r="Z117" s="45"/>
       <c r="AA117" s="9" t="s">
         <v>125</v>
       </c>
@@ -22989,7 +23046,7 @@
       </c>
     </row>
     <row r="118" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z118" s="39"/>
+      <c r="Z118" s="45"/>
       <c r="AA118" s="9" t="s">
         <v>126</v>
       </c>
@@ -23025,7 +23082,7 @@
       </c>
     </row>
     <row r="119" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z119" s="39"/>
+      <c r="Z119" s="45"/>
       <c r="AA119" s="9" t="s">
         <v>127</v>
       </c>
@@ -23061,7 +23118,7 @@
       </c>
     </row>
     <row r="120" spans="26:37" ht="24" x14ac:dyDescent="0.2">
-      <c r="Z120" s="39"/>
+      <c r="Z120" s="45"/>
       <c r="AA120" s="9" t="s">
         <v>128</v>
       </c>
@@ -23097,7 +23154,7 @@
       </c>
     </row>
     <row r="121" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z121" s="39"/>
+      <c r="Z121" s="45"/>
       <c r="AA121" s="9" t="s">
         <v>129</v>
       </c>
@@ -23133,7 +23190,7 @@
       </c>
     </row>
     <row r="122" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z122" s="39"/>
+      <c r="Z122" s="45"/>
       <c r="AA122" s="9" t="s">
         <v>130</v>
       </c>
@@ -23168,8 +23225,8 @@
         <v>1.3685261741000001</v>
       </c>
     </row>
-    <row r="123" spans="26:37" ht="36" x14ac:dyDescent="0.2">
-      <c r="Z123" s="39"/>
+    <row r="123" spans="26:37" ht="48" x14ac:dyDescent="0.2">
+      <c r="Z123" s="45"/>
       <c r="AA123" s="9" t="s">
         <v>131</v>
       </c>
@@ -23205,7 +23262,7 @@
       </c>
     </row>
     <row r="124" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z124" s="39"/>
+      <c r="Z124" s="45"/>
       <c r="AA124" s="9" t="s">
         <v>132</v>
       </c>
@@ -23241,7 +23298,7 @@
       </c>
     </row>
     <row r="125" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z125" s="39"/>
+      <c r="Z125" s="45"/>
       <c r="AA125" s="9" t="s">
         <v>133</v>
       </c>
@@ -23277,7 +23334,7 @@
       </c>
     </row>
     <row r="126" spans="26:37" ht="24" x14ac:dyDescent="0.2">
-      <c r="Z126" s="39"/>
+      <c r="Z126" s="45"/>
       <c r="AA126" s="10" t="s">
         <v>134</v>
       </c>
@@ -23313,7 +23370,7 @@
       </c>
     </row>
     <row r="127" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z127" s="39"/>
+      <c r="Z127" s="45"/>
       <c r="AA127" s="9" t="s">
         <v>135</v>
       </c>
@@ -23349,7 +23406,7 @@
       </c>
     </row>
     <row r="128" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z128" s="39"/>
+      <c r="Z128" s="45"/>
       <c r="AA128" s="9" t="s">
         <v>136</v>
       </c>
@@ -23385,7 +23442,7 @@
       </c>
     </row>
     <row r="129" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z129" s="39"/>
+      <c r="Z129" s="45"/>
       <c r="AA129" s="9" t="s">
         <v>137</v>
       </c>
@@ -23421,7 +23478,7 @@
       </c>
     </row>
     <row r="130" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z130" s="39"/>
+      <c r="Z130" s="45"/>
       <c r="AA130" s="9" t="s">
         <v>138</v>
       </c>
@@ -23457,7 +23514,7 @@
       </c>
     </row>
     <row r="131" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z131" s="39"/>
+      <c r="Z131" s="45"/>
       <c r="AA131" s="9" t="s">
         <v>139</v>
       </c>
@@ -23493,7 +23550,7 @@
       </c>
     </row>
     <row r="132" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z132" s="39"/>
+      <c r="Z132" s="45"/>
       <c r="AA132" s="9" t="s">
         <v>140</v>
       </c>
@@ -23529,7 +23586,7 @@
       </c>
     </row>
     <row r="133" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z133" s="39"/>
+      <c r="Z133" s="45"/>
       <c r="AA133" s="9" t="s">
         <v>141</v>
       </c>
@@ -23565,7 +23622,7 @@
       </c>
     </row>
     <row r="134" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z134" s="39"/>
+      <c r="Z134" s="45"/>
       <c r="AA134" s="9" t="s">
         <v>142</v>
       </c>
@@ -23601,7 +23658,7 @@
       </c>
     </row>
     <row r="135" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z135" s="39"/>
+      <c r="Z135" s="45"/>
       <c r="AA135" s="9" t="s">
         <v>143</v>
       </c>
@@ -23637,7 +23694,7 @@
       </c>
     </row>
     <row r="136" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z136" s="39"/>
+      <c r="Z136" s="45"/>
       <c r="AA136" s="10" t="s">
         <v>144</v>
       </c>
@@ -23673,7 +23730,7 @@
       </c>
     </row>
     <row r="137" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z137" s="39"/>
+      <c r="Z137" s="45"/>
       <c r="AA137" s="9" t="s">
         <v>145</v>
       </c>
@@ -23709,7 +23766,7 @@
       </c>
     </row>
     <row r="138" spans="26:37" ht="48" x14ac:dyDescent="0.2">
-      <c r="Z138" s="39"/>
+      <c r="Z138" s="45"/>
       <c r="AA138" s="9" t="s">
         <v>146</v>
       </c>
@@ -23745,7 +23802,7 @@
       </c>
     </row>
     <row r="139" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z139" s="39"/>
+      <c r="Z139" s="45"/>
       <c r="AA139" s="9" t="s">
         <v>147</v>
       </c>
@@ -23781,7 +23838,7 @@
       </c>
     </row>
     <row r="140" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z140" s="39"/>
+      <c r="Z140" s="45"/>
       <c r="AA140" s="9" t="s">
         <v>148</v>
       </c>
@@ -23817,7 +23874,7 @@
       </c>
     </row>
     <row r="141" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z141" s="39"/>
+      <c r="Z141" s="45"/>
       <c r="AA141" s="10" t="s">
         <v>149</v>
       </c>
@@ -23852,8 +23909,8 @@
         <v>3.6095629051999998</v>
       </c>
     </row>
-    <row r="142" spans="26:37" ht="36" x14ac:dyDescent="0.2">
-      <c r="Z142" s="39"/>
+    <row r="142" spans="26:37" ht="48" x14ac:dyDescent="0.2">
+      <c r="Z142" s="45"/>
       <c r="AA142" s="9" t="s">
         <v>150</v>
       </c>
@@ -23889,7 +23946,7 @@
       </c>
     </row>
     <row r="143" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z143" s="39"/>
+      <c r="Z143" s="45"/>
       <c r="AA143" s="9" t="s">
         <v>151</v>
       </c>
@@ -23925,7 +23982,7 @@
       </c>
     </row>
     <row r="144" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z144" s="39"/>
+      <c r="Z144" s="45"/>
       <c r="AA144" s="9" t="s">
         <v>152</v>
       </c>
@@ -23961,7 +24018,7 @@
       </c>
     </row>
     <row r="145" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z145" s="39"/>
+      <c r="Z145" s="45"/>
       <c r="AA145" s="9" t="s">
         <v>153</v>
       </c>
@@ -23997,7 +24054,7 @@
       </c>
     </row>
     <row r="146" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z146" s="39"/>
+      <c r="Z146" s="45"/>
       <c r="AA146" s="9" t="s">
         <v>154</v>
       </c>
@@ -24033,7 +24090,7 @@
       </c>
     </row>
     <row r="147" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z147" s="39"/>
+      <c r="Z147" s="45"/>
       <c r="AA147" s="9" t="s">
         <v>155</v>
       </c>
@@ -24069,7 +24126,7 @@
       </c>
     </row>
     <row r="148" spans="26:37" ht="24" x14ac:dyDescent="0.2">
-      <c r="Z148" s="39"/>
+      <c r="Z148" s="45"/>
       <c r="AA148" s="10" t="s">
         <v>156</v>
       </c>
@@ -24105,7 +24162,7 @@
       </c>
     </row>
     <row r="149" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z149" s="39"/>
+      <c r="Z149" s="45"/>
       <c r="AA149" s="9" t="s">
         <v>157</v>
       </c>
@@ -24141,7 +24198,7 @@
       </c>
     </row>
     <row r="150" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z150" s="39"/>
+      <c r="Z150" s="45"/>
       <c r="AA150" s="9" t="s">
         <v>158</v>
       </c>
@@ -24177,7 +24234,7 @@
       </c>
     </row>
     <row r="151" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z151" s="39"/>
+      <c r="Z151" s="45"/>
       <c r="AA151" s="9" t="s">
         <v>159</v>
       </c>
@@ -24213,7 +24270,7 @@
       </c>
     </row>
     <row r="152" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z152" s="39"/>
+      <c r="Z152" s="45"/>
       <c r="AA152" s="9" t="s">
         <v>160</v>
       </c>
@@ -24249,7 +24306,7 @@
       </c>
     </row>
     <row r="153" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z153" s="39"/>
+      <c r="Z153" s="45"/>
       <c r="AA153" s="9" t="s">
         <v>161</v>
       </c>
@@ -24285,7 +24342,7 @@
       </c>
     </row>
     <row r="154" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z154" s="39"/>
+      <c r="Z154" s="45"/>
       <c r="AA154" s="9" t="s">
         <v>162</v>
       </c>
@@ -24321,7 +24378,7 @@
       </c>
     </row>
     <row r="155" spans="26:37" ht="24" x14ac:dyDescent="0.2">
-      <c r="Z155" s="39"/>
+      <c r="Z155" s="45"/>
       <c r="AA155" s="10" t="s">
         <v>163</v>
       </c>
@@ -24357,7 +24414,7 @@
       </c>
     </row>
     <row r="156" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z156" s="39"/>
+      <c r="Z156" s="45"/>
       <c r="AA156" s="9" t="s">
         <v>164</v>
       </c>
@@ -24393,7 +24450,7 @@
       </c>
     </row>
     <row r="157" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z157" s="39"/>
+      <c r="Z157" s="45"/>
       <c r="AA157" s="9" t="s">
         <v>165</v>
       </c>
@@ -24429,7 +24486,7 @@
       </c>
     </row>
     <row r="158" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z158" s="39"/>
+      <c r="Z158" s="45"/>
       <c r="AA158" s="10" t="s">
         <v>166</v>
       </c>
@@ -24465,7 +24522,7 @@
       </c>
     </row>
     <row r="159" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z159" s="39"/>
+      <c r="Z159" s="45"/>
       <c r="AA159" s="10" t="s">
         <v>167</v>
       </c>
@@ -24501,7 +24558,7 @@
       </c>
     </row>
     <row r="160" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z160" s="39"/>
+      <c r="Z160" s="45"/>
       <c r="AA160" s="9" t="s">
         <v>168</v>
       </c>
@@ -24537,7 +24594,7 @@
       </c>
     </row>
     <row r="161" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z161" s="39"/>
+      <c r="Z161" s="45"/>
       <c r="AA161" s="9" t="s">
         <v>169</v>
       </c>
@@ -24573,7 +24630,7 @@
       </c>
     </row>
     <row r="162" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z162" s="39"/>
+      <c r="Z162" s="45"/>
       <c r="AA162" s="9" t="s">
         <v>170</v>
       </c>
@@ -24609,7 +24666,7 @@
       </c>
     </row>
     <row r="163" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z163" s="39"/>
+      <c r="Z163" s="45"/>
       <c r="AA163" s="9" t="s">
         <v>171</v>
       </c>
@@ -24645,7 +24702,7 @@
       </c>
     </row>
     <row r="164" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z164" s="39"/>
+      <c r="Z164" s="45"/>
       <c r="AA164" s="9" t="s">
         <v>172</v>
       </c>
@@ -24681,7 +24738,7 @@
       </c>
     </row>
     <row r="165" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z165" s="39"/>
+      <c r="Z165" s="45"/>
       <c r="AA165" s="10" t="s">
         <v>173</v>
       </c>
@@ -24717,7 +24774,7 @@
       </c>
     </row>
     <row r="166" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z166" s="39"/>
+      <c r="Z166" s="45"/>
       <c r="AA166" s="9" t="s">
         <v>174</v>
       </c>
@@ -24753,7 +24810,7 @@
       </c>
     </row>
     <row r="167" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z167" s="39"/>
+      <c r="Z167" s="45"/>
       <c r="AA167" s="9" t="s">
         <v>175</v>
       </c>
@@ -24789,7 +24846,7 @@
       </c>
     </row>
     <row r="168" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z168" s="39"/>
+      <c r="Z168" s="45"/>
       <c r="AA168" s="9" t="s">
         <v>176</v>
       </c>
@@ -24825,7 +24882,7 @@
       </c>
     </row>
     <row r="169" spans="26:37" ht="24" x14ac:dyDescent="0.2">
-      <c r="Z169" s="39"/>
+      <c r="Z169" s="45"/>
       <c r="AA169" s="10" t="s">
         <v>177</v>
       </c>
@@ -24861,7 +24918,7 @@
       </c>
     </row>
     <row r="170" spans="26:37" ht="24" x14ac:dyDescent="0.2">
-      <c r="Z170" s="39"/>
+      <c r="Z170" s="45"/>
       <c r="AA170" s="9" t="s">
         <v>178</v>
       </c>
@@ -24897,7 +24954,7 @@
       </c>
     </row>
     <row r="171" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z171" s="39"/>
+      <c r="Z171" s="45"/>
       <c r="AA171" s="9" t="s">
         <v>179</v>
       </c>
@@ -24933,7 +24990,7 @@
       </c>
     </row>
     <row r="172" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z172" s="39"/>
+      <c r="Z172" s="45"/>
       <c r="AA172" s="9" t="s">
         <v>180</v>
       </c>
@@ -24969,7 +25026,7 @@
       </c>
     </row>
     <row r="173" spans="26:37" ht="24" x14ac:dyDescent="0.2">
-      <c r="Z173" s="39"/>
+      <c r="Z173" s="45"/>
       <c r="AA173" s="9" t="s">
         <v>181</v>
       </c>
@@ -25005,7 +25062,7 @@
       </c>
     </row>
     <row r="174" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z174" s="39"/>
+      <c r="Z174" s="45"/>
       <c r="AA174" s="9" t="s">
         <v>182</v>
       </c>
@@ -25041,7 +25098,7 @@
       </c>
     </row>
     <row r="175" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z175" s="39"/>
+      <c r="Z175" s="45"/>
       <c r="AA175" s="9" t="s">
         <v>183</v>
       </c>
@@ -25077,7 +25134,7 @@
       </c>
     </row>
     <row r="176" spans="26:37" ht="24" x14ac:dyDescent="0.2">
-      <c r="Z176" s="39"/>
+      <c r="Z176" s="45"/>
       <c r="AA176" s="9" t="s">
         <v>184</v>
       </c>
@@ -25113,7 +25170,7 @@
       </c>
     </row>
     <row r="177" spans="26:37" ht="36" x14ac:dyDescent="0.2">
-      <c r="Z177" s="39"/>
+      <c r="Z177" s="45"/>
       <c r="AA177" s="10" t="s">
         <v>185</v>
       </c>
@@ -25149,7 +25206,7 @@
       </c>
     </row>
     <row r="178" spans="26:37" ht="60" x14ac:dyDescent="0.2">
-      <c r="Z178" s="39"/>
+      <c r="Z178" s="45"/>
       <c r="AA178" s="9" t="s">
         <v>186</v>
       </c>
@@ -25185,7 +25242,7 @@
       </c>
     </row>
     <row r="179" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z179" s="39"/>
+      <c r="Z179" s="45"/>
       <c r="AA179" s="9" t="s">
         <v>187</v>
       </c>
@@ -25221,7 +25278,7 @@
       </c>
     </row>
     <row r="180" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z180" s="39"/>
+      <c r="Z180" s="45"/>
       <c r="AA180" s="9" t="s">
         <v>188</v>
       </c>
@@ -25257,7 +25314,7 @@
       </c>
     </row>
     <row r="181" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z181" s="39"/>
+      <c r="Z181" s="45"/>
       <c r="AA181" s="10" t="s">
         <v>189</v>
       </c>
@@ -25293,7 +25350,7 @@
       </c>
     </row>
     <row r="182" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z182" s="39"/>
+      <c r="Z182" s="45"/>
       <c r="AA182" s="9" t="s">
         <v>190</v>
       </c>
@@ -25329,7 +25386,7 @@
       </c>
     </row>
     <row r="183" spans="26:37" ht="24" x14ac:dyDescent="0.2">
-      <c r="Z183" s="39"/>
+      <c r="Z183" s="45"/>
       <c r="AA183" s="9" t="s">
         <v>191</v>
       </c>
@@ -25365,7 +25422,7 @@
       </c>
     </row>
     <row r="184" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z184" s="39"/>
+      <c r="Z184" s="45"/>
       <c r="AA184" s="9" t="s">
         <v>192</v>
       </c>
@@ -25401,7 +25458,7 @@
       </c>
     </row>
     <row r="185" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z185" s="39"/>
+      <c r="Z185" s="45"/>
       <c r="AA185" s="9" t="s">
         <v>193</v>
       </c>
@@ -25437,7 +25494,7 @@
       </c>
     </row>
     <row r="186" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z186" s="39"/>
+      <c r="Z186" s="45"/>
       <c r="AA186" s="9" t="s">
         <v>194</v>
       </c>
@@ -25473,7 +25530,7 @@
       </c>
     </row>
     <row r="187" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z187" s="39"/>
+      <c r="Z187" s="45"/>
       <c r="AA187" s="9" t="s">
         <v>195</v>
       </c>
@@ -25509,7 +25566,7 @@
       </c>
     </row>
     <row r="188" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z188" s="39"/>
+      <c r="Z188" s="45"/>
       <c r="AA188" s="9" t="s">
         <v>196</v>
       </c>
@@ -25545,7 +25602,7 @@
       </c>
     </row>
     <row r="189" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z189" s="39"/>
+      <c r="Z189" s="45"/>
       <c r="AA189" s="9" t="s">
         <v>197</v>
       </c>
@@ -25581,7 +25638,7 @@
       </c>
     </row>
     <row r="190" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z190" s="39"/>
+      <c r="Z190" s="45"/>
       <c r="AA190" s="9" t="s">
         <v>198</v>
       </c>
@@ -25617,7 +25674,7 @@
       </c>
     </row>
     <row r="191" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z191" s="39"/>
+      <c r="Z191" s="45"/>
       <c r="AA191" s="9" t="s">
         <v>199</v>
       </c>
@@ -25653,7 +25710,7 @@
       </c>
     </row>
     <row r="192" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z192" s="39"/>
+      <c r="Z192" s="45"/>
       <c r="AA192" s="9" t="s">
         <v>200</v>
       </c>
@@ -25689,7 +25746,7 @@
       </c>
     </row>
     <row r="193" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z193" s="39"/>
+      <c r="Z193" s="45"/>
       <c r="AA193" s="9" t="s">
         <v>201</v>
       </c>
@@ -25725,7 +25782,7 @@
       </c>
     </row>
     <row r="194" spans="26:37" ht="24" x14ac:dyDescent="0.2">
-      <c r="Z194" s="39"/>
+      <c r="Z194" s="45"/>
       <c r="AA194" s="9" t="s">
         <v>202</v>
       </c>
@@ -25761,7 +25818,7 @@
       </c>
     </row>
     <row r="195" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z195" s="39"/>
+      <c r="Z195" s="45"/>
       <c r="AA195" s="9" t="s">
         <v>203</v>
       </c>
@@ -25797,7 +25854,7 @@
       </c>
     </row>
     <row r="196" spans="26:37" ht="24" x14ac:dyDescent="0.2">
-      <c r="Z196" s="39"/>
+      <c r="Z196" s="45"/>
       <c r="AA196" s="9" t="s">
         <v>204</v>
       </c>
@@ -25832,8 +25889,8 @@
         <v>11.8604651163</v>
       </c>
     </row>
-    <row r="197" spans="26:37" ht="36" x14ac:dyDescent="0.2">
-      <c r="Z197" s="39"/>
+    <row r="197" spans="26:37" ht="48" x14ac:dyDescent="0.2">
+      <c r="Z197" s="45"/>
       <c r="AA197" s="9" t="s">
         <v>205</v>
       </c>
@@ -25869,7 +25926,7 @@
       </c>
     </row>
     <row r="198" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z198" s="39"/>
+      <c r="Z198" s="45"/>
       <c r="AA198" s="9" t="s">
         <v>206</v>
       </c>
@@ -25905,7 +25962,7 @@
       </c>
     </row>
     <row r="199" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z199" s="39"/>
+      <c r="Z199" s="45"/>
       <c r="AA199" s="9" t="s">
         <v>207</v>
       </c>
@@ -25941,7 +25998,7 @@
       </c>
     </row>
     <row r="200" spans="26:37" ht="24" x14ac:dyDescent="0.2">
-      <c r="Z200" s="39"/>
+      <c r="Z200" s="45"/>
       <c r="AA200" s="9" t="s">
         <v>208</v>
       </c>
@@ -25977,7 +26034,7 @@
       </c>
     </row>
     <row r="201" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z201" s="39"/>
+      <c r="Z201" s="45"/>
       <c r="AA201" s="9" t="s">
         <v>209</v>
       </c>
@@ -26013,7 +26070,7 @@
       </c>
     </row>
     <row r="202" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z202" s="39"/>
+      <c r="Z202" s="45"/>
       <c r="AA202" s="9" t="s">
         <v>210</v>
       </c>
@@ -26049,7 +26106,7 @@
       </c>
     </row>
     <row r="203" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z203" s="39"/>
+      <c r="Z203" s="45"/>
       <c r="AA203" s="9" t="s">
         <v>211</v>
       </c>
@@ -26085,7 +26142,7 @@
       </c>
     </row>
     <row r="204" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z204" s="39"/>
+      <c r="Z204" s="45"/>
       <c r="AA204" s="9" t="s">
         <v>212</v>
       </c>
@@ -26121,7 +26178,7 @@
       </c>
     </row>
     <row r="205" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z205" s="39"/>
+      <c r="Z205" s="45"/>
       <c r="AA205" s="9" t="s">
         <v>213</v>
       </c>
@@ -26157,7 +26214,7 @@
       </c>
     </row>
     <row r="206" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z206" s="39"/>
+      <c r="Z206" s="45"/>
       <c r="AA206" s="9" t="s">
         <v>214</v>
       </c>
@@ -26193,7 +26250,7 @@
       </c>
     </row>
     <row r="207" spans="26:37" ht="24" x14ac:dyDescent="0.2">
-      <c r="Z207" s="39"/>
+      <c r="Z207" s="45"/>
       <c r="AA207" s="9" t="s">
         <v>215</v>
       </c>
@@ -26229,7 +26286,7 @@
       </c>
     </row>
     <row r="208" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z208" s="39"/>
+      <c r="Z208" s="45"/>
       <c r="AA208" s="9" t="s">
         <v>216</v>
       </c>
@@ -26265,7 +26322,7 @@
       </c>
     </row>
     <row r="209" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z209" s="39"/>
+      <c r="Z209" s="45"/>
       <c r="AA209" s="9" t="s">
         <v>217</v>
       </c>
@@ -26301,7 +26358,7 @@
       </c>
     </row>
     <row r="210" spans="26:37" ht="60" x14ac:dyDescent="0.2">
-      <c r="Z210" s="39"/>
+      <c r="Z210" s="45"/>
       <c r="AA210" s="9" t="s">
         <v>218</v>
       </c>
@@ -26337,7 +26394,7 @@
       </c>
     </row>
     <row r="211" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z211" s="39"/>
+      <c r="Z211" s="45"/>
       <c r="AA211" s="9" t="s">
         <v>219</v>
       </c>
@@ -26373,7 +26430,7 @@
       </c>
     </row>
     <row r="212" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z212" s="39"/>
+      <c r="Z212" s="45"/>
       <c r="AA212" s="9" t="s">
         <v>220</v>
       </c>
@@ -26409,7 +26466,7 @@
       </c>
     </row>
     <row r="213" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z213" s="39"/>
+      <c r="Z213" s="45"/>
       <c r="AA213" s="9" t="s">
         <v>221</v>
       </c>
@@ -26445,7 +26502,7 @@
       </c>
     </row>
     <row r="214" spans="26:37" ht="36" x14ac:dyDescent="0.2">
-      <c r="Z214" s="39"/>
+      <c r="Z214" s="45"/>
       <c r="AA214" s="9" t="s">
         <v>222</v>
       </c>
@@ -26481,7 +26538,7 @@
       </c>
     </row>
     <row r="215" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z215" s="39"/>
+      <c r="Z215" s="45"/>
       <c r="AA215" s="9" t="s">
         <v>223</v>
       </c>
@@ -26517,7 +26574,7 @@
       </c>
     </row>
     <row r="216" spans="26:37" ht="24" x14ac:dyDescent="0.2">
-      <c r="Z216" s="39"/>
+      <c r="Z216" s="45"/>
       <c r="AA216" s="9" t="s">
         <v>224</v>
       </c>
@@ -26553,7 +26610,7 @@
       </c>
     </row>
     <row r="217" spans="26:37" ht="24" x14ac:dyDescent="0.2">
-      <c r="Z217" s="39"/>
+      <c r="Z217" s="45"/>
       <c r="AA217" s="9" t="s">
         <v>225</v>
       </c>
@@ -26589,7 +26646,7 @@
       </c>
     </row>
     <row r="218" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z218" s="39"/>
+      <c r="Z218" s="45"/>
       <c r="AA218" s="10" t="s">
         <v>226</v>
       </c>
@@ -26625,7 +26682,7 @@
       </c>
     </row>
     <row r="219" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z219" s="39"/>
+      <c r="Z219" s="45"/>
       <c r="AA219" s="9" t="s">
         <v>227</v>
       </c>
@@ -26661,7 +26718,7 @@
       </c>
     </row>
     <row r="220" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z220" s="39"/>
+      <c r="Z220" s="45"/>
       <c r="AA220" s="9" t="s">
         <v>228</v>
       </c>
@@ -26697,7 +26754,7 @@
       </c>
     </row>
     <row r="221" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z221" s="39"/>
+      <c r="Z221" s="45"/>
       <c r="AA221" s="10" t="s">
         <v>229</v>
       </c>
@@ -26733,7 +26790,7 @@
       </c>
     </row>
     <row r="222" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z222" s="39"/>
+      <c r="Z222" s="45"/>
       <c r="AA222" s="9" t="s">
         <v>230</v>
       </c>
@@ -26769,7 +26826,7 @@
       </c>
     </row>
     <row r="223" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z223" s="39"/>
+      <c r="Z223" s="45"/>
       <c r="AA223" s="9" t="s">
         <v>231</v>
       </c>
@@ -26805,7 +26862,7 @@
       </c>
     </row>
     <row r="224" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z224" s="39"/>
+      <c r="Z224" s="45"/>
       <c r="AA224" s="9" t="s">
         <v>232</v>
       </c>
@@ -26841,7 +26898,7 @@
       </c>
     </row>
     <row r="225" spans="26:37" ht="24" x14ac:dyDescent="0.2">
-      <c r="Z225" s="39"/>
+      <c r="Z225" s="45"/>
       <c r="AA225" s="9" t="s">
         <v>233</v>
       </c>
@@ -26877,7 +26934,7 @@
       </c>
     </row>
     <row r="226" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z226" s="39"/>
+      <c r="Z226" s="45"/>
       <c r="AA226" s="9" t="s">
         <v>234</v>
       </c>
@@ -26913,7 +26970,7 @@
       </c>
     </row>
     <row r="227" spans="26:37" ht="24" x14ac:dyDescent="0.2">
-      <c r="Z227" s="39"/>
+      <c r="Z227" s="45"/>
       <c r="AA227" s="10" t="s">
         <v>235</v>
       </c>
@@ -26949,7 +27006,7 @@
       </c>
     </row>
     <row r="228" spans="26:37" ht="24" x14ac:dyDescent="0.2">
-      <c r="Z228" s="39"/>
+      <c r="Z228" s="45"/>
       <c r="AA228" s="9" t="s">
         <v>236</v>
       </c>
@@ -26985,7 +27042,7 @@
       </c>
     </row>
     <row r="229" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z229" s="39"/>
+      <c r="Z229" s="45"/>
       <c r="AA229" s="9" t="s">
         <v>237</v>
       </c>
@@ -27021,7 +27078,7 @@
       </c>
     </row>
     <row r="230" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z230" s="39"/>
+      <c r="Z230" s="45"/>
       <c r="AA230" s="9" t="s">
         <v>238</v>
       </c>
@@ -27057,7 +27114,7 @@
       </c>
     </row>
     <row r="231" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z231" s="39"/>
+      <c r="Z231" s="45"/>
       <c r="AA231" s="9" t="s">
         <v>239</v>
       </c>
@@ -27093,7 +27150,7 @@
       </c>
     </row>
     <row r="232" spans="26:37" ht="24" x14ac:dyDescent="0.2">
-      <c r="Z232" s="39"/>
+      <c r="Z232" s="45"/>
       <c r="AA232" s="9" t="s">
         <v>240</v>
       </c>
@@ -27129,7 +27186,7 @@
       </c>
     </row>
     <row r="233" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z233" s="39"/>
+      <c r="Z233" s="45"/>
       <c r="AA233" s="9" t="s">
         <v>241</v>
       </c>
@@ -27165,7 +27222,7 @@
       </c>
     </row>
     <row r="234" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z234" s="39"/>
+      <c r="Z234" s="45"/>
       <c r="AA234" s="10" t="s">
         <v>242</v>
       </c>
@@ -27201,7 +27258,7 @@
       </c>
     </row>
     <row r="235" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z235" s="39"/>
+      <c r="Z235" s="45"/>
       <c r="AA235" s="9" t="s">
         <v>243</v>
       </c>
@@ -27237,7 +27294,7 @@
       </c>
     </row>
     <row r="236" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z236" s="39"/>
+      <c r="Z236" s="45"/>
       <c r="AA236" s="9" t="s">
         <v>244</v>
       </c>
@@ -27273,7 +27330,7 @@
       </c>
     </row>
     <row r="237" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z237" s="39"/>
+      <c r="Z237" s="45"/>
       <c r="AA237" s="9" t="s">
         <v>245</v>
       </c>
@@ -27309,7 +27366,7 @@
       </c>
     </row>
     <row r="238" spans="26:37" ht="36" x14ac:dyDescent="0.2">
-      <c r="Z238" s="39"/>
+      <c r="Z238" s="45"/>
       <c r="AA238" s="9" t="s">
         <v>246</v>
       </c>
@@ -27345,7 +27402,7 @@
       </c>
     </row>
     <row r="239" spans="26:37" ht="24" x14ac:dyDescent="0.2">
-      <c r="Z239" s="39"/>
+      <c r="Z239" s="45"/>
       <c r="AA239" s="9" t="s">
         <v>247</v>
       </c>
@@ -27381,7 +27438,7 @@
       </c>
     </row>
     <row r="240" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z240" s="39"/>
+      <c r="Z240" s="45"/>
       <c r="AA240" s="10" t="s">
         <v>248</v>
       </c>
@@ -27417,7 +27474,7 @@
       </c>
     </row>
     <row r="241" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z241" s="39"/>
+      <c r="Z241" s="45"/>
       <c r="AA241" s="9" t="s">
         <v>249</v>
       </c>
@@ -27453,7 +27510,7 @@
       </c>
     </row>
     <row r="242" spans="26:37" x14ac:dyDescent="0.2">
-      <c r="Z242" s="40"/>
+      <c r="Z242" s="46"/>
       <c r="AA242" s="9" t="s">
         <v>250</v>
       </c>
@@ -27490,39 +27547,114 @@
     </row>
   </sheetData>
   <mergeCells count="165">
-    <mergeCell ref="BP17:BQ17"/>
-    <mergeCell ref="BP18:BQ18"/>
-    <mergeCell ref="BP19:BQ19"/>
-    <mergeCell ref="BP20:BQ20"/>
-    <mergeCell ref="BP21:BQ21"/>
-    <mergeCell ref="BP11:BQ11"/>
-    <mergeCell ref="BP12:BQ12"/>
-    <mergeCell ref="BP13:BQ13"/>
-    <mergeCell ref="BP14:BQ14"/>
-    <mergeCell ref="BP15:BQ15"/>
-    <mergeCell ref="BP16:BQ16"/>
-    <mergeCell ref="BP2:BR2"/>
-    <mergeCell ref="BP3:BQ3"/>
-    <mergeCell ref="BP4:BQ4"/>
-    <mergeCell ref="BP5:BQ5"/>
-    <mergeCell ref="BP6:BQ6"/>
-    <mergeCell ref="BP7:BQ7"/>
-    <mergeCell ref="BP8:BQ8"/>
-    <mergeCell ref="BP9:BQ9"/>
-    <mergeCell ref="BP10:BQ10"/>
-    <mergeCell ref="BA21:BB21"/>
-    <mergeCell ref="BA15:BB15"/>
-    <mergeCell ref="BA16:BB16"/>
-    <mergeCell ref="BA17:BB17"/>
-    <mergeCell ref="BA18:BB18"/>
-    <mergeCell ref="BA19:BB19"/>
-    <mergeCell ref="BA20:BB20"/>
-    <mergeCell ref="BA9:BB9"/>
-    <mergeCell ref="BA10:BB10"/>
-    <mergeCell ref="BA11:BB11"/>
-    <mergeCell ref="BA12:BB12"/>
-    <mergeCell ref="BA13:BB13"/>
-    <mergeCell ref="BA14:BB14"/>
+    <mergeCell ref="Z11:AA11"/>
+    <mergeCell ref="Z12:AA12"/>
+    <mergeCell ref="Z13:AA13"/>
+    <mergeCell ref="Z2:AB2"/>
+    <mergeCell ref="Z3:AA3"/>
+    <mergeCell ref="Z4:AA4"/>
+    <mergeCell ref="Z5:AA5"/>
+    <mergeCell ref="Z6:AA6"/>
+    <mergeCell ref="Z7:AA7"/>
+    <mergeCell ref="Z46:Z242"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="Z37:AA37"/>
+    <mergeCell ref="Z38:AA38"/>
+    <mergeCell ref="Z39:AA39"/>
+    <mergeCell ref="Z40:AA40"/>
+    <mergeCell ref="Z41:AA41"/>
+    <mergeCell ref="Z42:AA42"/>
+    <mergeCell ref="Z31:AA31"/>
+    <mergeCell ref="Z32:AA32"/>
+    <mergeCell ref="Z33:AA33"/>
+    <mergeCell ref="Z34:AA34"/>
+    <mergeCell ref="Z35:AA35"/>
+    <mergeCell ref="Z36:AA36"/>
+    <mergeCell ref="Z25:AA25"/>
+    <mergeCell ref="Z26:AA26"/>
+    <mergeCell ref="Z27:AA27"/>
+    <mergeCell ref="Z28:AA28"/>
+    <mergeCell ref="Z29:AA29"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="R2:S2"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="X2:Y2"/>
+    <mergeCell ref="Z43:AA43"/>
+    <mergeCell ref="Z44:AA44"/>
+    <mergeCell ref="Z45:AA45"/>
+    <mergeCell ref="Z30:AA30"/>
+    <mergeCell ref="Z20:AA20"/>
+    <mergeCell ref="Z21:AA21"/>
+    <mergeCell ref="Z22:AA22"/>
+    <mergeCell ref="Z23:AA23"/>
+    <mergeCell ref="Z24:AA24"/>
+    <mergeCell ref="Z14:AA14"/>
+    <mergeCell ref="Z15:AA15"/>
+    <mergeCell ref="Z16:AA16"/>
+    <mergeCell ref="Z17:AA17"/>
+    <mergeCell ref="Z18:AA18"/>
+    <mergeCell ref="Z19:AA19"/>
+    <mergeCell ref="Z8:AA8"/>
+    <mergeCell ref="Z9:AA9"/>
+    <mergeCell ref="Z10:AA10"/>
+    <mergeCell ref="T3:U3"/>
+    <mergeCell ref="V3:W3"/>
+    <mergeCell ref="X3:Y3"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="R3:S3"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="AL8:AM8"/>
+    <mergeCell ref="AL9:AM9"/>
+    <mergeCell ref="AL10:AM10"/>
+    <mergeCell ref="AL11:AM11"/>
+    <mergeCell ref="AL12:AM12"/>
+    <mergeCell ref="AL13:AM13"/>
+    <mergeCell ref="AL2:AN2"/>
+    <mergeCell ref="AL3:AM3"/>
+    <mergeCell ref="AL4:AM4"/>
+    <mergeCell ref="AL5:AM5"/>
+    <mergeCell ref="AL6:AM6"/>
+    <mergeCell ref="AL7:AM7"/>
+    <mergeCell ref="AL22:AM22"/>
+    <mergeCell ref="AL23:AM23"/>
+    <mergeCell ref="AL24:AM24"/>
+    <mergeCell ref="AL14:AM14"/>
+    <mergeCell ref="AL15:AM15"/>
+    <mergeCell ref="AL16:AM16"/>
+    <mergeCell ref="AL17:AM17"/>
+    <mergeCell ref="AL18:AM18"/>
+    <mergeCell ref="AL19:AM19"/>
     <mergeCell ref="AL37:AM37"/>
     <mergeCell ref="AL38:AM38"/>
     <mergeCell ref="AL39:AM39"/>
@@ -27547,114 +27679,39 @@
     <mergeCell ref="AL30:AM30"/>
     <mergeCell ref="AL20:AM20"/>
     <mergeCell ref="AL21:AM21"/>
-    <mergeCell ref="AL22:AM22"/>
-    <mergeCell ref="AL23:AM23"/>
-    <mergeCell ref="AL24:AM24"/>
-    <mergeCell ref="AL14:AM14"/>
-    <mergeCell ref="AL15:AM15"/>
-    <mergeCell ref="AL16:AM16"/>
-    <mergeCell ref="AL17:AM17"/>
-    <mergeCell ref="AL18:AM18"/>
-    <mergeCell ref="AL19:AM19"/>
-    <mergeCell ref="AL8:AM8"/>
-    <mergeCell ref="AL9:AM9"/>
-    <mergeCell ref="AL10:AM10"/>
-    <mergeCell ref="AL11:AM11"/>
-    <mergeCell ref="AL12:AM12"/>
-    <mergeCell ref="AL13:AM13"/>
-    <mergeCell ref="AL2:AN2"/>
-    <mergeCell ref="AL3:AM3"/>
-    <mergeCell ref="AL4:AM4"/>
-    <mergeCell ref="AL5:AM5"/>
-    <mergeCell ref="AL6:AM6"/>
-    <mergeCell ref="AL7:AM7"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="R3:S3"/>
-    <mergeCell ref="T3:U3"/>
-    <mergeCell ref="V3:W3"/>
-    <mergeCell ref="X3:Y3"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="R2:S2"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="X2:Y2"/>
-    <mergeCell ref="Z43:AA43"/>
-    <mergeCell ref="Z44:AA44"/>
-    <mergeCell ref="Z45:AA45"/>
-    <mergeCell ref="Z30:AA30"/>
-    <mergeCell ref="Z20:AA20"/>
-    <mergeCell ref="Z21:AA21"/>
-    <mergeCell ref="Z22:AA22"/>
-    <mergeCell ref="Z23:AA23"/>
-    <mergeCell ref="Z24:AA24"/>
-    <mergeCell ref="Z14:AA14"/>
-    <mergeCell ref="Z15:AA15"/>
-    <mergeCell ref="Z16:AA16"/>
-    <mergeCell ref="Z17:AA17"/>
-    <mergeCell ref="Z18:AA18"/>
-    <mergeCell ref="Z19:AA19"/>
-    <mergeCell ref="Z8:AA8"/>
-    <mergeCell ref="Z9:AA9"/>
-    <mergeCell ref="Z10:AA10"/>
-    <mergeCell ref="Z46:Z242"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="Z37:AA37"/>
-    <mergeCell ref="Z38:AA38"/>
-    <mergeCell ref="Z39:AA39"/>
-    <mergeCell ref="Z40:AA40"/>
-    <mergeCell ref="Z41:AA41"/>
-    <mergeCell ref="Z42:AA42"/>
-    <mergeCell ref="Z31:AA31"/>
-    <mergeCell ref="Z32:AA32"/>
-    <mergeCell ref="Z33:AA33"/>
-    <mergeCell ref="Z34:AA34"/>
-    <mergeCell ref="Z35:AA35"/>
-    <mergeCell ref="Z36:AA36"/>
-    <mergeCell ref="Z25:AA25"/>
-    <mergeCell ref="Z26:AA26"/>
-    <mergeCell ref="Z27:AA27"/>
-    <mergeCell ref="Z28:AA28"/>
-    <mergeCell ref="Z29:AA29"/>
-    <mergeCell ref="Z11:AA11"/>
-    <mergeCell ref="Z12:AA12"/>
-    <mergeCell ref="Z13:AA13"/>
-    <mergeCell ref="Z2:AB2"/>
-    <mergeCell ref="Z3:AA3"/>
-    <mergeCell ref="Z4:AA4"/>
-    <mergeCell ref="Z5:AA5"/>
-    <mergeCell ref="Z6:AA6"/>
-    <mergeCell ref="Z7:AA7"/>
+    <mergeCell ref="BA21:BB21"/>
+    <mergeCell ref="BA15:BB15"/>
+    <mergeCell ref="BA16:BB16"/>
+    <mergeCell ref="BA17:BB17"/>
+    <mergeCell ref="BA18:BB18"/>
+    <mergeCell ref="BA19:BB19"/>
+    <mergeCell ref="BA20:BB20"/>
+    <mergeCell ref="BA9:BB9"/>
+    <mergeCell ref="BA10:BB10"/>
+    <mergeCell ref="BA11:BB11"/>
+    <mergeCell ref="BA12:BB12"/>
+    <mergeCell ref="BA13:BB13"/>
+    <mergeCell ref="BA14:BB14"/>
+    <mergeCell ref="BP2:BR2"/>
+    <mergeCell ref="BP3:BQ3"/>
+    <mergeCell ref="BP4:BQ4"/>
+    <mergeCell ref="BP5:BQ5"/>
+    <mergeCell ref="BP6:BQ6"/>
+    <mergeCell ref="BP7:BQ7"/>
+    <mergeCell ref="BP8:BQ8"/>
+    <mergeCell ref="BP9:BQ9"/>
+    <mergeCell ref="BP10:BQ10"/>
+    <mergeCell ref="BP17:BQ17"/>
+    <mergeCell ref="BP18:BQ18"/>
+    <mergeCell ref="BP19:BQ19"/>
+    <mergeCell ref="BP20:BQ20"/>
+    <mergeCell ref="BP21:BQ21"/>
+    <mergeCell ref="BP11:BQ11"/>
+    <mergeCell ref="BP12:BQ12"/>
+    <mergeCell ref="BP13:BQ13"/>
+    <mergeCell ref="BP14:BQ14"/>
+    <mergeCell ref="BP15:BQ15"/>
+    <mergeCell ref="BP16:BQ16"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="Z16" r:id="rId1" display="http://stats.oecd.org/OECDStat_Metadata/ShowMetadata.ashx?Dataset=LAND_COVER&amp;Coords=[COU].[DEU]&amp;ShowOnWeb=true&amp;Lang=en" xr:uid="{BCABFC22-D90F-6F45-82A6-33F4A19DDEEE}"/>
@@ -28954,8 +29011,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3A052B2-06A9-E34E-A0E1-58BBD5827602}">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>